<commit_message>
Recommend Exercise work Successfully
</commit_message>
<xml_diff>
--- a/exercise_recommendation_bmi_expanded.xlsx
+++ b/exercise_recommendation_bmi_expanded.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\smartgym\SmartGym-Major\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="T:\Smart_Gym_Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{497AE824-DBAB-4214-989F-1730BFB2D3C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73C7F225-EE43-4B5E-96AD-142E6AFB6A1C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -710,8 +710,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>